<commit_message>
whole run use expansion affective words
</commit_message>
<xml_diff>
--- a/log/result.xlsx
+++ b/log/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Valence" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="23">
   <si>
     <t>Methods</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,6 +101,12 @@
     <t>ml_geo_tfidf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>使用扩增情感词汇</t>
+  </si>
+  <si>
+    <t>ml_pos_neg_geo</t>
+  </si>
 </sst>
 </file>
 
@@ -151,9 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -490,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:G15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -503,9 +513,10 @@
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +538,32 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -550,8 +585,30 @@
       <c r="G2">
         <v>1.62600709321439</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="3"/>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>2.2895740711300001</v>
+      </c>
+      <c r="M2">
+        <v>1.2650509963100001</v>
+      </c>
+      <c r="N2">
+        <v>0.61395709257900799</v>
+      </c>
+      <c r="O2">
+        <v>0.22016400612299999</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.63349443994688504</v>
+      </c>
+      <c r="Q2">
+        <v>1.5131338576384901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -573,8 +630,30 @@
       <c r="G3">
         <v>1.6874675035551101</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" s="3"/>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>2.4425592146700001</v>
+      </c>
+      <c r="M3">
+        <v>1.29428470009</v>
+      </c>
+      <c r="N3">
+        <v>0.53472680265873396</v>
+      </c>
+      <c r="O3">
+        <v>0.16805679414800001</v>
+      </c>
+      <c r="P3">
+        <v>0.56854979563544195</v>
+      </c>
+      <c r="Q3">
+        <v>1.5628689051445199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -596,8 +675,30 @@
       <c r="G4">
         <v>1.6031880076990599</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" s="3"/>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>2.30483546429</v>
+      </c>
+      <c r="M4">
+        <v>1.2543727711499999</v>
+      </c>
+      <c r="N4">
+        <v>0.55100890988617601</v>
+      </c>
+      <c r="O4">
+        <v>0.21496592851900001</v>
+      </c>
+      <c r="P4">
+        <v>0.58759274893353097</v>
+      </c>
+      <c r="Q4">
+        <v>1.5181684571517799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -619,8 +720,30 @@
       <c r="G5">
         <v>1.51807176790188</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5" s="3"/>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>2.1289918818800002</v>
+      </c>
+      <c r="M5">
+        <v>1.2355209041799999</v>
+      </c>
+      <c r="N5">
+        <v>0.61943402548787296</v>
+      </c>
+      <c r="O5">
+        <v>0.27485879531200003</v>
+      </c>
+      <c r="P5">
+        <v>0.63945848603317401</v>
+      </c>
+      <c r="Q5">
+        <v>1.4591065354800401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -642,8 +765,30 @@
       <c r="G6">
         <v>1.5302731604698001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" s="3"/>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>2.17261484961</v>
+      </c>
+      <c r="M6">
+        <v>1.2291270279399999</v>
+      </c>
+      <c r="N6">
+        <v>0.55373753156044903</v>
+      </c>
+      <c r="O6">
+        <v>0.26000067789100001</v>
+      </c>
+      <c r="P6">
+        <v>0.59024557724148996</v>
+      </c>
+      <c r="Q6">
+        <v>1.4739792568446499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -665,8 +810,30 @@
       <c r="G7">
         <v>1.5938977504634699</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" s="3"/>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>2.2889488314699999</v>
+      </c>
+      <c r="M7">
+        <v>1.2662129198900001</v>
+      </c>
+      <c r="N7">
+        <v>0.54036642812936297</v>
+      </c>
+      <c r="O7">
+        <v>0.220376964679</v>
+      </c>
+      <c r="P7">
+        <v>0.57477649190870195</v>
+      </c>
+      <c r="Q7">
+        <v>1.5129272393195099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -688,8 +855,30 @@
       <c r="G8">
         <v>1.3753217086396201</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8" s="3"/>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>1.9476701868199999</v>
+      </c>
+      <c r="M8">
+        <v>1.1588053839400001</v>
+      </c>
+      <c r="N8">
+        <v>0.612030873885543</v>
+      </c>
+      <c r="O8">
+        <v>-0.34654548727000001</v>
+      </c>
+      <c r="P8">
+        <v>0.62372105240026998</v>
+      </c>
+      <c r="Q8">
+        <v>1.3955895481204399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -711,8 +900,30 @@
       <c r="G9">
         <v>1.4323486764672899</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" s="3"/>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9">
+        <v>2.0507498400699999</v>
+      </c>
+      <c r="M9">
+        <v>1.17679100406</v>
+      </c>
+      <c r="N9">
+        <v>0.58324826809126495</v>
+      </c>
+      <c r="O9">
+        <v>-0.57620779398199995</v>
+      </c>
+      <c r="P9">
+        <v>0.58808220368136699</v>
+      </c>
+      <c r="Q9">
+        <v>1.43204393789699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -734,8 +945,30 @@
       <c r="G10">
         <v>1.6438907659818001</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I10" s="3"/>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>2.7155357847200001</v>
+      </c>
+      <c r="M10">
+        <v>1.39816044168</v>
+      </c>
+      <c r="N10">
+        <v>0.35345456361954602</v>
+      </c>
+      <c r="O10">
+        <v>-9.2142289779500004</v>
+      </c>
+      <c r="P10">
+        <v>0.31710675652141501</v>
+      </c>
+      <c r="Q10">
+        <v>1.64788828041096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -757,8 +990,30 @@
       <c r="G11">
         <v>1.4229510619347401</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="I11" s="3"/>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>2.2050337123800001</v>
+      </c>
+      <c r="M11">
+        <v>1.2603103153399999</v>
+      </c>
+      <c r="N11">
+        <v>0.54041830717765005</v>
+      </c>
+      <c r="O11">
+        <v>-1.0638593113899999</v>
+      </c>
+      <c r="P11">
+        <v>0.56120786290038505</v>
+      </c>
+      <c r="Q11">
+        <v>1.4849355919960801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -780,8 +1035,30 @@
       <c r="G12">
         <v>1.4012282869692001</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="I12" s="3"/>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12">
+        <v>2.1305619166800001</v>
+      </c>
+      <c r="M12">
+        <v>1.21365960075</v>
+      </c>
+      <c r="N12">
+        <v>0.55943728228676903</v>
+      </c>
+      <c r="O12">
+        <v>-0.87668747609200004</v>
+      </c>
+      <c r="P12">
+        <v>0.58320655675236199</v>
+      </c>
+      <c r="Q12">
+        <v>1.4596444487195399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -803,8 +1080,30 @@
       <c r="G13">
         <v>1.36831976105887</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="I13" s="3"/>
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1.9125905807600001</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1.1526593038299999</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.62050887372163599</v>
+      </c>
+      <c r="O13">
+        <v>-0.32349675173800002</v>
+      </c>
+      <c r="P13">
+        <v>0.63621565131108104</v>
+      </c>
+      <c r="Q13">
+        <v>1.3829644177505001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -826,8 +1125,30 @@
       <c r="G14">
         <v>1.4154578213793501</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="I14" s="3"/>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14">
+        <v>2.1858091991999999</v>
+      </c>
+      <c r="M14">
+        <v>1.25691025237</v>
+      </c>
+      <c r="N14">
+        <v>0.54526157837823697</v>
+      </c>
+      <c r="O14">
+        <v>-1.0363734503099999</v>
+      </c>
+      <c r="P14">
+        <v>0.57341305820123001</v>
+      </c>
+      <c r="Q14">
+        <v>1.4784482402835</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -849,8 +1170,77 @@
       <c r="G15">
         <v>1.4017304169881799</v>
       </c>
+      <c r="I15" s="3"/>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <v>2.1158114397499999</v>
+      </c>
+      <c r="M15">
+        <v>1.2157992385</v>
+      </c>
+      <c r="N15">
+        <v>0.56252031743042197</v>
+      </c>
+      <c r="O15">
+        <v>-0.89736377801300005</v>
+      </c>
+      <c r="P15">
+        <v>0.58487464700424696</v>
+      </c>
+      <c r="Q15">
+        <v>1.4545829092029201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>2.3197667156400001</v>
+      </c>
+      <c r="C16">
+        <v>1.2842367692000001</v>
+      </c>
+      <c r="D16">
+        <v>0.50244305000748302</v>
+      </c>
+      <c r="E16">
+        <v>-2.0440276369400001</v>
+      </c>
+      <c r="F16">
+        <v>0.49794854834038499</v>
+      </c>
+      <c r="G16">
+        <v>1.52307803990433</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16">
+        <v>2.2428662128300001</v>
+      </c>
+      <c r="M16">
+        <v>1.3128813404699999</v>
+      </c>
+      <c r="N16">
+        <v>0.53046381600165904</v>
+      </c>
+      <c r="O16">
+        <v>-1.9589599359500001</v>
+      </c>
+      <c r="P16">
+        <v>0.54404462103158502</v>
+      </c>
+      <c r="Q16">
+        <v>1.4976201831001199</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:I15"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -859,18 +1249,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:G15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,8 +1283,32 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -915,8 +1330,30 @@
       <c r="G2">
         <v>1.16045573809395</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="3"/>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>1.3092978958599999</v>
+      </c>
+      <c r="M2">
+        <v>0.91924611273199996</v>
+      </c>
+      <c r="N2">
+        <v>0.29884867737280701</v>
+      </c>
+      <c r="O2">
+        <v>7.4003076706799994E-2</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.276134417810454</v>
+      </c>
+      <c r="Q2">
+        <v>1.1442455575000099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -938,8 +1375,30 @@
       <c r="G3">
         <v>1.1829696396805101</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" s="3"/>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>1.34121802376</v>
+      </c>
+      <c r="M3">
+        <v>0.92474203297699997</v>
+      </c>
+      <c r="N3">
+        <v>0.26762969315790103</v>
+      </c>
+      <c r="O3">
+        <v>5.1427664099700003E-2</v>
+      </c>
+      <c r="P3">
+        <v>0.24777069649307801</v>
+      </c>
+      <c r="Q3">
+        <v>1.1581096769117001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -961,8 +1420,30 @@
       <c r="G4">
         <v>1.19465666725258</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" s="3"/>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>1.34324076726</v>
+      </c>
+      <c r="M4">
+        <v>0.92606570331399995</v>
+      </c>
+      <c r="N4">
+        <v>0.28522318008080999</v>
+      </c>
+      <c r="O4">
+        <v>4.9997084959200001E-2</v>
+      </c>
+      <c r="P4">
+        <v>0.26828753146085998</v>
+      </c>
+      <c r="Q4">
+        <v>1.1589826432080601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -984,8 +1465,30 @@
       <c r="G5">
         <v>1.1593302688667999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5" s="3"/>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>1.30561463753</v>
+      </c>
+      <c r="M5">
+        <v>0.91702866816999995</v>
+      </c>
+      <c r="N5">
+        <v>0.28755558213111598</v>
+      </c>
+      <c r="O5">
+        <v>7.6608049866099995E-2</v>
+      </c>
+      <c r="P5">
+        <v>0.26480899926773699</v>
+      </c>
+      <c r="Q5">
+        <v>1.1426349537512299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1007,8 +1510,30 @@
       <c r="G6">
         <v>1.19123071710008</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" s="3"/>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>1.33540966509</v>
+      </c>
+      <c r="M6">
+        <v>0.92264886697600001</v>
+      </c>
+      <c r="N6">
+        <v>0.27793922298819601</v>
+      </c>
+      <c r="O6">
+        <v>5.5535607962400001E-2</v>
+      </c>
+      <c r="P6">
+        <v>0.26029393755750402</v>
+      </c>
+      <c r="Q6">
+        <v>1.1555992666529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1030,8 +1555,30 @@
       <c r="G7">
         <v>1.1835513236069499</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" s="3"/>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>1.3387133198800001</v>
+      </c>
+      <c r="M7">
+        <v>0.92353163683100004</v>
+      </c>
+      <c r="N7">
+        <v>0.25897818211302398</v>
+      </c>
+      <c r="O7">
+        <v>5.3199108236500002E-2</v>
+      </c>
+      <c r="P7">
+        <v>0.23830274436096699</v>
+      </c>
+      <c r="Q7">
+        <v>1.15702779563964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1053,8 +1600,30 @@
       <c r="G8">
         <v>1.1089460628899701</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8" s="3"/>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>1.24303707581</v>
+      </c>
+      <c r="M8">
+        <v>0.89791690687400005</v>
+      </c>
+      <c r="N8">
+        <v>0.29505177039758701</v>
+      </c>
+      <c r="O8">
+        <v>-10.4802085504</v>
+      </c>
+      <c r="P8">
+        <v>0.25794795145298499</v>
+      </c>
+      <c r="Q8">
+        <v>1.1149157258767699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1076,8 +1645,30 @@
       <c r="G9">
         <v>1.0951911356641999</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" s="3"/>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9">
+        <v>1.21183314239</v>
+      </c>
+      <c r="M9">
+        <v>0.88075573611799995</v>
+      </c>
+      <c r="N9">
+        <v>0.33309139074764099</v>
+      </c>
+      <c r="O9">
+        <v>-8.93166373605</v>
+      </c>
+      <c r="P9">
+        <v>0.289266441530525</v>
+      </c>
+      <c r="Q9">
+        <v>1.10083293118697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1099,8 +1690,30 @@
       <c r="G10">
         <v>1.1224659258768701</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I10" s="3"/>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <v>1.25596559811</v>
+      </c>
+      <c r="M10">
+        <v>0.90534653291199996</v>
+      </c>
+      <c r="N10">
+        <v>0.278997420571446</v>
+      </c>
+      <c r="O10">
+        <v>-9.2047417774000007</v>
+      </c>
+      <c r="P10">
+        <v>0.23808788481610499</v>
+      </c>
+      <c r="Q10">
+        <v>1.12069870978292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1122,8 +1735,30 @@
       <c r="G11">
         <v>1.11068664751742</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="I11" s="3"/>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>1.26281398278</v>
+      </c>
+      <c r="M11">
+        <v>0.89175815099599998</v>
+      </c>
+      <c r="N11">
+        <v>0.27102643600891801</v>
+      </c>
+      <c r="O11">
+        <v>-9.9282950404400001</v>
+      </c>
+      <c r="P11">
+        <v>0.230691238212172</v>
+      </c>
+      <c r="Q11">
+        <v>1.1237499645287801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1145,8 +1780,30 @@
       <c r="G12">
         <v>1.10951297132814</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="I12" s="3"/>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12">
+        <v>1.2491694233699999</v>
+      </c>
+      <c r="M12">
+        <v>0.89372232693499998</v>
+      </c>
+      <c r="N12">
+        <v>0.28773353760627002</v>
+      </c>
+      <c r="O12">
+        <v>-9.4863830389900006</v>
+      </c>
+      <c r="P12">
+        <v>0.25146237309963698</v>
+      </c>
+      <c r="Q12">
+        <v>1.1176624818646801</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1168,8 +1825,30 @@
       <c r="G13">
         <v>1.1184612310583399</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="I13" s="3"/>
+      <c r="K13" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1.2637225949899999</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.90867437101899995</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.267770642452695</v>
+      </c>
+      <c r="O13">
+        <v>-11.736576210999999</v>
+      </c>
+      <c r="P13">
+        <v>0.236129718232054</v>
+      </c>
+      <c r="Q13">
+        <v>1.12415416869259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1191,8 +1870,30 @@
       <c r="G14">
         <v>1.11733871974554</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="I14" s="3"/>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14">
+        <v>1.2757172633</v>
+      </c>
+      <c r="M14">
+        <v>0.89976179091700004</v>
+      </c>
+      <c r="N14">
+        <v>0.25361640839615901</v>
+      </c>
+      <c r="O14">
+        <v>-10.808322716299999</v>
+      </c>
+      <c r="P14">
+        <v>0.207337528740247</v>
+      </c>
+      <c r="Q14">
+        <v>1.1294765439332899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1214,8 +1915,77 @@
       <c r="G15">
         <v>1.1150935583873101</v>
       </c>
+      <c r="I15" s="3"/>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <v>1.2604895136400001</v>
+      </c>
+      <c r="M15">
+        <v>0.90115402783200005</v>
+      </c>
+      <c r="N15">
+        <v>0.272983483329168</v>
+      </c>
+      <c r="O15">
+        <v>-10.3087572401</v>
+      </c>
+      <c r="P15">
+        <v>0.246671044065122</v>
+      </c>
+      <c r="Q15">
+        <v>1.12271524156435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>1.0829469443499999</v>
+      </c>
+      <c r="C16">
+        <v>0.83595465867300001</v>
+      </c>
+      <c r="D16">
+        <v>0.459190531874273</v>
+      </c>
+      <c r="E16">
+        <v>-3.3750506110299998</v>
+      </c>
+      <c r="F16">
+        <v>0.42522527694081302</v>
+      </c>
+      <c r="G16">
+        <v>1.0406473679155701</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16">
+        <v>1.1023366532600001</v>
+      </c>
+      <c r="M16">
+        <v>0.83526136472500001</v>
+      </c>
+      <c r="N16">
+        <v>0.44547173610457103</v>
+      </c>
+      <c r="O16">
+        <v>-3.8801456077199998</v>
+      </c>
+      <c r="P16">
+        <v>0.42167514096506598</v>
+      </c>
+      <c r="Q16">
+        <v>1.0499222129582499</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:I15"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1226,7 +1996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add more experiment record
</commit_message>
<xml_diff>
--- a/log/result.xlsx
+++ b/log/result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="33">
   <si>
     <t>Methods</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,6 +106,36 @@
   </si>
   <si>
     <t>ml_pos_neg_geo</t>
+  </si>
+  <si>
+    <t>使用word embeddings</t>
+  </si>
+  <si>
+    <t>average of word vecs</t>
+  </si>
+  <si>
+    <t>alpha = 1</t>
+  </si>
+  <si>
+    <t>alpha = 2.5</t>
+  </si>
+  <si>
+    <t>Bayesian Ridge Regression</t>
+  </si>
+  <si>
+    <t>SVR</t>
+  </si>
+  <si>
+    <t>Knn Regression</t>
+  </si>
+  <si>
+    <t>Doc2vec</t>
+  </si>
+  <si>
+    <t>epoch = 100</t>
+  </si>
+  <si>
+    <t>More big corpus</t>
   </si>
 </sst>
 </file>
@@ -157,12 +187,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,746 +548,930 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="6" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="6"/>
+    <col min="11" max="11" width="17.7109375" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" ht="30">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>2.64389906718</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>1.31356359535</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>0.62015643970921197</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>9.9479819078899995E-2</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="8">
         <v>0.623778875942408</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="6">
         <v>1.62600709321439</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="K2" t="s">
+      <c r="I2" s="7"/>
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="6">
         <v>2.2895740711300001</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="6">
         <v>1.2650509963100001</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="6">
         <v>0.61395709257900799</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="6">
         <v>0.22016400612299999</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="9">
         <v>0.63349443994688504</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="6">
         <v>1.5131338576384901</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>2.84754657555</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>1.35018373115</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>0.58441149042942397</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>3.0116849304999999E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>0.58722291123104098</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>1.6874675035551101</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="K3" t="s">
+      <c r="I3" s="7"/>
+      <c r="K3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="6">
         <v>2.4425592146700001</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="6">
         <v>1.29428470009</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="6">
         <v>0.53472680265873396</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="6">
         <v>0.16805679414800001</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="6">
         <v>0.56854979563544195</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="6">
         <v>1.5628689051445199</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>2.5702117880299999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>1.27697865293</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>0.59253757760665404</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>0.12457793374499999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>0.59081127885078899</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>1.6031880076990599</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="K4" t="s">
+      <c r="I4" s="7"/>
+      <c r="K4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="6">
         <v>2.30483546429</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="6">
         <v>1.2543727711499999</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="6">
         <v>0.55100890988617601</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="6">
         <v>0.21496592851900001</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="6">
         <v>0.58759274893353097</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="6">
         <v>1.5181684571517799</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>2.3045418925000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>1.2293371470700001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>0.62230253353893406</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>0.215065919976</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>0.61805349309271496</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="6">
         <v>1.51807176790188</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="K5" t="s">
+      <c r="I5" s="7"/>
+      <c r="K5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="6">
         <v>2.1289918818800002</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="6">
         <v>1.2355209041799999</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="6">
         <v>0.61943402548787296</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="6">
         <v>0.27485879531200003</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="6">
         <v>0.63945848603317401</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="6">
         <v>1.4591065354800401</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>2.34173594565</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>1.21747315829</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>0.59295470477479795</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>0.20239751069799999</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>0.58679604144581099</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>1.5302731604698001</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="K6" t="s">
+      <c r="I6" s="7"/>
+      <c r="K6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="6">
         <v>2.17261484961</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="6">
         <v>1.2291270279399999</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="6">
         <v>0.55373753156044903</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="6">
         <v>0.26000067789100001</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="6">
         <v>0.59024557724148996</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="6">
         <v>1.4739792568446499</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>2.5405100389299999</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>1.2735847387400001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>0.59006166898114099</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>0.134694441143</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>0.58550565042789204</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>1.5938977504634699</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="K7" t="s">
+      <c r="I7" s="7"/>
+      <c r="K7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="6">
         <v>2.2889488314699999</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="6">
         <v>1.2662129198900001</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="6">
         <v>0.54036642812936297</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="6">
         <v>0.220376964679</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="6">
         <v>0.57477649190870195</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="6">
         <v>1.5129272393195099</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>1.8915098022600001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>1.13981921319</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0.62552186700729495</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>-0.35283621016900002</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>0.60460085064920299</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <v>1.3753217086396201</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="K8" t="s">
+      <c r="I8" s="7"/>
+      <c r="K8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="6">
         <v>1.9476701868199999</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="6">
         <v>1.1588053839400001</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="6">
         <v>0.612030873885543</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="6">
         <v>-0.34654548727000001</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="6">
         <v>0.62372105240026998</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="6">
         <v>1.3955895481204399</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>2.0516227309800001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>1.19977359579</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>0.58672136429729904</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>-0.52877498998799999</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>0.58765388908598004</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>1.4323486764672899</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="K9" t="s">
+      <c r="I9" s="7"/>
+      <c r="K9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="6">
         <v>2.0507498400699999</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="6">
         <v>1.17679100406</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="6">
         <v>0.58324826809126495</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="6">
         <v>-0.57620779398199995</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="6">
         <v>0.58808220368136699</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="6">
         <v>1.43204393789699</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>2.7023768504799999</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>1.40259034114</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>0.36392105471390901</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>-9.0772284789299995</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>0.31841146831173101</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>1.6438907659818001</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="K10" t="s">
+      <c r="I10" s="7"/>
+      <c r="K10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="6">
         <v>2.7155357847200001</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="6">
         <v>1.39816044168</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="6">
         <v>0.35345456361954602</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="6">
         <v>-9.2142289779500004</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="6">
         <v>0.31710675652141501</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="6">
         <v>1.64788828041096</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>2.0247897246600002</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>1.20302831392</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>0.58936525651321103</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>-0.73821266550300002</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>0.57870842031022596</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>1.4229510619347401</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="K11" t="s">
+      <c r="I11" s="7"/>
+      <c r="K11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="6">
         <v>2.2050337123800001</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="6">
         <v>1.2603103153399999</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="6">
         <v>0.54041830717765005</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="6">
         <v>-1.0638593113899999</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="6">
         <v>0.56120786290038505</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="6">
         <v>1.4849355919960801</v>
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <v>1.9634407121999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>1.1688750059999999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>0.604531550302851</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>-0.66528426487000003</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>0.58479945175394399</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>1.4012282869692001</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="K12" t="s">
+      <c r="I12" s="7"/>
+      <c r="K12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="6">
         <v>2.1305619166800001</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="6">
         <v>1.21365960075</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="6">
         <v>0.55943728228676903</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="6">
         <v>-0.87668747609200004</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="6">
         <v>0.58320655675236199</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="6">
         <v>1.4596444487195399</v>
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="8">
         <v>1.8722989685</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="8">
         <v>1.13062805659</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="8">
         <v>0.629243729309375</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <v>-0.38105389464799999</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <v>0.60778016979226301</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="6">
         <v>1.36831976105887</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="K13" t="s">
+      <c r="I13" s="7"/>
+      <c r="K13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="8">
         <v>1.9125905807600001</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="8">
         <v>1.1526593038299999</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="8">
         <v>0.62050887372163599</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="6">
         <v>-0.32349675173800002</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="6">
         <v>0.63621565131108104</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="6">
         <v>1.3829644177505001</v>
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <v>2.0035208441000001</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>1.19918616292</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <v>0.59406367277202499</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <v>-0.75406007075000003</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <v>0.57770185892113901</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <v>1.4154578213793501</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="K14" t="s">
+      <c r="I14" s="7"/>
+      <c r="K14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="6">
         <v>2.1858091991999999</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="6">
         <v>1.25691025237</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="6">
         <v>0.54526157837823697</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="6">
         <v>-1.0363734503099999</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="6">
         <v>0.57341305820123001</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="6">
         <v>1.4784482402835</v>
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>1.96484816191</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>1.16964297555</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>0.60350602520861396</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>-0.70709525543399998</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="6">
         <v>0.58351203834065901</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="6">
         <v>1.4017304169881799</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="K15" t="s">
+      <c r="I15" s="7"/>
+      <c r="K15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="6">
         <v>2.1158114397499999</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="6">
         <v>1.2157992385</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="6">
         <v>0.56252031743042197</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="6">
         <v>-0.89736377801300005</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="6">
         <v>0.58487464700424696</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="6">
         <v>1.4545829092029201</v>
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
         <v>2.3197667156400001</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>1.2842367692000001</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>0.50244305000748302</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>-2.0440276369400001</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="6">
         <v>0.49794854834038499</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="6">
         <v>1.52307803990433</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="6">
         <v>2.2428662128300001</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="6">
         <v>1.3128813404699999</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="6">
         <v>0.53046381600165904</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="6">
         <v>-1.9589599359500001</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="6">
         <v>0.54404462103158502</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="6">
         <v>1.4976201831001199</v>
       </c>
     </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="30">
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1.48597012572</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.98113486020700003</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.72443800083867804</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-1.4918710468800001E-2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.72757876317942405</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1.2190037431121501</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="6">
+        <v>1.5316235094299999</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.99809170019799998</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.72187822390220502</v>
+      </c>
+      <c r="E21" s="6">
+        <v>-0.34891889625</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.72334824513096696</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1.2375877784762399</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30">
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6">
+        <v>1.4899518006100001</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.97777936492100004</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.72348397180167801</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.117923588782</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.73587098050385802</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1.22063581817425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1.4941718295599999</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.97886813403700002</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.71781997672106002</v>
+      </c>
+      <c r="E23" s="6">
+        <v>-1.35759564187E-2</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.725070598559721</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1.22236321507209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1.6186562574500001</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.98807338911099996</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.69125207177367198</v>
+      </c>
+      <c r="E24" s="6">
+        <v>-4.1545245404099998E-2</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.68582626319999496</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1.2722642247006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1.84873228175</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1.11854738692</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.64180949045065905</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-0.28771992511099997</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.64840275888630405</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1.3596809485116099</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1.71173646261</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1.0993277156300001</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.75625652437047197</v>
+      </c>
+      <c r="E26" s="6">
+        <v>-2.3156178438600001</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.77548912885978905</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1.3083334676643299</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I1:I15"/>
+    <mergeCell ref="A19:G19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1249,15 +1481,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1283,7 +1521,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="K1" t="s">
@@ -1330,7 +1568,7 @@
       <c r="G2">
         <v>1.16045573809395</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="4"/>
       <c r="K2" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1613,7 @@
       <c r="G3">
         <v>1.1829696396805101</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="4"/>
       <c r="K3" t="s">
         <v>8</v>
       </c>
@@ -1420,7 +1658,7 @@
       <c r="G4">
         <v>1.19465666725258</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="4"/>
       <c r="K4" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1703,7 @@
       <c r="G5">
         <v>1.1593302688667999</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="4"/>
       <c r="K5" t="s">
         <v>10</v>
       </c>
@@ -1510,7 +1748,7 @@
       <c r="G6">
         <v>1.19123071710008</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="4"/>
       <c r="K6" t="s">
         <v>11</v>
       </c>
@@ -1555,7 +1793,7 @@
       <c r="G7">
         <v>1.1835513236069499</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="4"/>
       <c r="K7" t="s">
         <v>12</v>
       </c>
@@ -1600,7 +1838,7 @@
       <c r="G8">
         <v>1.1089460628899701</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="4"/>
       <c r="K8" t="s">
         <v>13</v>
       </c>
@@ -1645,7 +1883,7 @@
       <c r="G9">
         <v>1.0951911356641999</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="4"/>
       <c r="K9" t="s">
         <v>14</v>
       </c>
@@ -1690,7 +1928,7 @@
       <c r="G10">
         <v>1.1224659258768701</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="4"/>
       <c r="K10" t="s">
         <v>15</v>
       </c>
@@ -1735,7 +1973,7 @@
       <c r="G11">
         <v>1.11068664751742</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="4"/>
       <c r="K11" t="s">
         <v>16</v>
       </c>
@@ -1780,7 +2018,7 @@
       <c r="G12">
         <v>1.10951297132814</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="4"/>
       <c r="K12" t="s">
         <v>17</v>
       </c>
@@ -1825,7 +2063,7 @@
       <c r="G13">
         <v>1.1184612310583399</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="4"/>
       <c r="K13" t="s">
         <v>18</v>
       </c>
@@ -1870,7 +2108,7 @@
       <c r="G14">
         <v>1.11733871974554</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="4"/>
       <c r="K14" t="s">
         <v>19</v>
       </c>
@@ -1915,7 +2153,7 @@
       <c r="G15">
         <v>1.1150935583873101</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="4"/>
       <c r="K15" t="s">
         <v>20</v>
       </c>
@@ -1982,9 +2220,189 @@
         <v>1.0499222129582499</v>
       </c>
     </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="A19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.98089295177900004</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.79276293491100003</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.534966090497349</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-1.5159584134299999</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.47967152601079199</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.99040039972662197</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" s="6">
+        <v>0.98361710095900001</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.79383009167999996</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.53948128026804198</v>
+      </c>
+      <c r="E21" s="6">
+        <v>-2.4773052408999998</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.48045333263597101</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0.99177472288771895</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30">
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>0.98141287563799995</v>
+      </c>
+      <c r="C22">
+        <v>0.79327279824200003</v>
+      </c>
+      <c r="D22">
+        <v>0.53461219842100205</v>
+      </c>
+      <c r="E22">
+        <v>-1.48931651372</v>
+      </c>
+      <c r="F22">
+        <v>0.47883947474389199</v>
+      </c>
+      <c r="G22">
+        <v>0.99066284660232196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>1.0024896873</v>
+      </c>
+      <c r="C23">
+        <v>0.80209781568399996</v>
+      </c>
+      <c r="D23">
+        <v>0.52617703998055898</v>
+      </c>
+      <c r="E23">
+        <v>-1.83209484158</v>
+      </c>
+      <c r="F23">
+        <v>0.48163106703791098</v>
+      </c>
+      <c r="G23">
+        <v>1.0012440697957901</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>0.99918690477799998</v>
+      </c>
+      <c r="C24">
+        <v>0.78856437065899998</v>
+      </c>
+      <c r="D24">
+        <v>0.52120134234067195</v>
+      </c>
+      <c r="E24">
+        <v>-1.13855751496</v>
+      </c>
+      <c r="F24">
+        <v>0.485745098302028</v>
+      </c>
+      <c r="G24">
+        <v>0.99959336971494295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>1.1469058275599999</v>
+      </c>
+      <c r="C25">
+        <v>0.85155102396399995</v>
+      </c>
+      <c r="D25">
+        <v>0.41431291864747599</v>
+      </c>
+      <c r="E25">
+        <v>-2.6977375058600002</v>
+      </c>
+      <c r="F25">
+        <v>0.41880717681563001</v>
+      </c>
+      <c r="G25">
+        <v>1.07093689242444</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>1.00600261972</v>
+      </c>
+      <c r="C26">
+        <v>0.79955083706100005</v>
+      </c>
+      <c r="D26">
+        <v>0.562279117979951</v>
+      </c>
+      <c r="E26">
+        <v>-5.62136095322</v>
+      </c>
+      <c r="F26">
+        <v>0.52936146688720098</v>
+      </c>
+      <c r="G26">
+        <v>1.00299681939452</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I1:I15"/>
+    <mergeCell ref="A19:H19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1997,7 +2415,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>